<commit_message>
On branch master Changes to be committed: 	modified:   tspi/ciclo-1/logt1/forma-logt1-20105627.xlsx 	deleted:    tspi/ciclo-1/logt2/forma-logt1-20105914.xlsx 	modified:   tspi/ciclo-1/logt2/forma-logt2-20105627.xlsx 	new file:   tspi/ciclo-1/logt2/forma-logt2-20105914.xlsx 	modified:   tspi/ciclo-1/reportessemanales.xlsx 	modified:   tspi/plan.xlsx
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/reportessemanales.xlsx
+++ b/tspi/ciclo-1/reportessemanales.xlsx
@@ -224,7 +224,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -368,11 +368,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="67637279"/>
-        <c:axId val="63148640"/>
+        <c:axId val="32104986"/>
+        <c:axId val="13293571"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67637279"/>
+        <c:axId val="32104986"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,7 +380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63148640"/>
+        <c:crossAx val="13293571"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -394,7 +394,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63148640"/>
+        <c:axId val="13293571"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -411,7 +411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67637279"/>
+        <c:crossAx val="32104986"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -443,7 +443,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -568,10 +568,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>NaN</c:v>
+                  <c:v>3.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>NaN</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>NaN</c:v>
@@ -580,18 +580,18 @@
                   <c:v>3.83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>NaN</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="77963178"/>
-        <c:axId val="86548636"/>
+        <c:axId val="74413454"/>
+        <c:axId val="90423527"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77963178"/>
+        <c:axId val="74413454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86548636"/>
+        <c:crossAx val="90423527"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -613,7 +613,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86548636"/>
+        <c:axId val="90423527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,7 +630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77963178"/>
+        <c:crossAx val="74413454"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -667,15 +667,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:colOff>81000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>22320</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:colOff>102240</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -683,8 +683,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="1508040"/>
-        <a:ext cx="10833120" cy="3573360"/>
+        <a:off x="81000" y="1180080"/>
+        <a:ext cx="10996560" cy="2884320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -702,15 +702,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:colOff>81000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>22320</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:colOff>102240</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -718,8 +718,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="1508040"/>
-        <a:ext cx="10833120" cy="3573360"/>
+        <a:off x="81000" y="1180080"/>
+        <a:ext cx="10996560" cy="2884320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -744,13 +744,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.9450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.5411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4039215686274"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.8117647058824"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -836,17 +836,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="C6"/>
+      <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.9450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.5411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4039215686274"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.8117647058824"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -864,7 +864,9 @@
       <c r="B2" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="n">
+        <v>3.92</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
       <c r="A3" s="3" t="s">
@@ -873,7 +875,9 @@
       <c r="B3" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="n">
+        <v>3.4</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
@@ -902,12 +906,14 @@
       <c r="B6" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="n">
+        <v>1.75</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Reporte semanal semana 2 ciclo 1
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/reportessemanales.xlsx
+++ b/tspi/ciclo-1/reportessemanales.xlsx
@@ -224,7 +224,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -368,11 +368,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="32104986"/>
-        <c:axId val="13293571"/>
+        <c:axId val="47165867"/>
+        <c:axId val="72352914"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="32104986"/>
+        <c:axId val="47165867"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,7 +380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="13293571"/>
+        <c:crossAx val="72352914"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -394,7 +394,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13293571"/>
+        <c:axId val="72352914"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -411,7 +411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="32104986"/>
+        <c:crossAx val="47165867"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -443,7 +443,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -574,7 +574,7 @@
                   <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>NaN</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3.83</c:v>
@@ -587,11 +587,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="74413454"/>
-        <c:axId val="90423527"/>
+        <c:axId val="10663870"/>
+        <c:axId val="22202762"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74413454"/>
+        <c:axId val="10663870"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90423527"/>
+        <c:crossAx val="22202762"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -613,7 +613,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90423527"/>
+        <c:axId val="22202762"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,7 +630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74413454"/>
+        <c:crossAx val="10663870"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -667,15 +667,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>117360</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:colOff>128880</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -683,8 +683,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="81000" y="1180080"/>
-        <a:ext cx="10996560" cy="2884320"/>
+        <a:off x="108000" y="1083600"/>
+        <a:ext cx="11048760" cy="2678760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -702,15 +702,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>117360</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:colOff>128880</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -718,8 +718,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="81000" y="1180080"/>
-        <a:ext cx="10996560" cy="2884320"/>
+        <a:off x="108000" y="1083600"/>
+        <a:ext cx="11048760" cy="2678760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -744,10 +744,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4039215686274"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5098039215686"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.443137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.0549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -836,14 +836,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
+      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4039215686274"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5098039215686"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.443137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.0549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -886,7 +886,9 @@
       <c r="B4" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
       <c r="A5" s="3" t="s">

</xml_diff>